<commit_message>
fixed a bug with mormelizing the book name
</commit_message>
<xml_diff>
--- a/excel/2015.xlsx
+++ b/excel/2015.xlsx
@@ -559,12 +559,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>20160101,20150101</t>
+          <t>20150101,20160101</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
     </row>
@@ -576,17 +576,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>בר, ניקו, 1955-  (דובר)  $$Qבר, ניקו, 1955-,בן יוסף, אורה  $$Qבן יוסף, אורה</t>
+          <t>בן יוסף, אורה  $$Qבן יוסף, אורה,בר, ניקו, 1955-  (דובר)  $$Qבר, ניקו, 1955-</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>גולדברג, לאה, 1911-1970 מחבר$$Qגולדברג, לאה, 1911-1970,גולדברג, לאה, 1911-1970$$Qגולדברג, לאה, 1911-1970</t>
+          <t>גולדברג, לאה, 1911-1970$$Qגולדברג, לאה, 1911-1970,גולדברג, לאה, 1911-1970 מחבר$$Qגולדברג, לאה, 1911-1970</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Hebrew literature -- Study and teaching,Children's stories, Hebrew</t>
+          <t>Children's stories, Hebrew,Hebrew literature -- Study and teaching</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -871,7 +871,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>הסוס הכי מהיר בעולם / נרי אלומה ; איורים - נעם נדב ; [עריכה - יונה טפר].,הסוס הכי מהיר בעולם / נרי אלומה ; מספר נרי אלומה.</t>
+          <t>הסוס הכי מהיר בעולם / נרי אלומה ; מספר נרי אלומה.,הסוס הכי מהיר בעולם / נרי אלומה ; איורים - נעם נדב ; [עריכה - יונה טפר].</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -886,12 +886,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21187644050005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361317010005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361317010005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21187644050005171</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>אלומה, נרי, 1963- מחבר דובר$$Qאלומה, נרי, 1963-,אלומה, נרי, 1963-$$Qאלומה, נרי, 1963-</t>
+          <t>אלומה, נרי, 1963-$$Qאלומה, נרי, 1963-,אלומה, נרי, 1963- מחבר דובר$$Qאלומה, נרי, 1963-</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -911,12 +911,12 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>20150101,20120101</t>
+          <t>20120101,20150101</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>בני ברק : הקיבוץ המאוחד,תל אביב : iCast</t>
+          <t>תל אביב : iCast,בני ברק : הקיבוץ המאוחד</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -931,7 +931,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ريپنكو، لينة  (رسام)  $$Qريپنكو، لينة,רבנקו, לנה  $$Qרבנקו, לנה</t>
+          <t>רבנקו, לנה  $$Qרבנקו, לנה,ريپنكو، لينة  (رسام)  $$Qريپنكو، لينة</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>34 ص.,34, [2] עמודים : איורים צבעוניים ; 22 ס"מ.</t>
+          <t>34, [2] עמודים : איורים צבעוניים ; 22 ס"מ.,34 ص.</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1040,7 +1040,7 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ara,heb</t>
+          <t>heb,ara</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1087,7 +1087,7 @@
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1200,12 +1200,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21256860510005171,NNL_ALEPH21182812720005171</t>
+          <t>NNL_ALEPH21182812720005171,NNL_ALEPH21256860510005171</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21182812720005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21256860510005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21256860510005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21182812720005171</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE79021020,https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE14746570</t>
+          <t>https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE14746570,https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE79021020</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1279,7 +1279,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>מהפחד הזה אני לא מפחד / עפרה גלברט אבני.,מהפחד הזה אני לא מפחד!. עפרה גלברט-אבני ; איורים - מישל קישקה ; [עריכה - יונה טפר].</t>
+          <t>מהפחד הזה אני לא מפחד!. עפרה גלברט-אבני ; איורים - מישל קישקה ; [עריכה - יונה טפר].,מהפחד הזה אני לא מפחד / עפרה גלברט אבני.</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21194309530005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11349306430005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11349306430005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21194309530005171</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1324,7 +1324,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>בני-ברק : הקיבוץ המאוחד,תל אביב : iCast</t>
+          <t>תל אביב : iCast,בני-ברק : הקיבוץ המאוחד</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -1371,7 +1371,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>$$VThe National Library of Israel$$ONNL_ALEPH21205138470005171,The National Library of Israel</t>
+          <t>The National Library of Israel,$$VThe National Library of Israel$$ONNL_ALEPH21205138470005171</t>
         </is>
       </c>
     </row>
@@ -1812,7 +1812,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>מאיר, מירה, 1932-2016  (מתרגם)  $$Qמאיר, מירה, 1932-2016,מאיר, מירה, 1932-2016  $$Qמאיר, מירה, 1932-2016</t>
+          <t>מאיר, מירה, 1932-2016  $$Qמאיר, מירה, 1932-2016,מאיר, מירה, 1932-2016  (מתרגם)  $$Qמאיר, מירה, 1932-2016</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1827,12 +1827,12 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>רוברטון, פיונה$$Qרוברטון, פיונה,רוברטון, פיונה מחבר מאייר$$Qרוברטון, פיונה</t>
+          <t>רוברטון, פיונה מחבר מאייר$$Qרוברטון, פיונה,רוברטון, פיונה$$Qרוברטון, פיונה</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Children's stories, English -- Translations into Hebrew; Pets -- Juvenile fiction; Friendship -- Juvenile fiction; Human-animal relationships -- Juvenile fiction,Children's stories, English -- 21st century; Children's stories -- Translations into Hebrew; Pets -- Juvenile fiction; Friendship -- Juvenile fiction; Human-animal relationships -- Juvenile fiction</t>
+          <t>Children's stories, English -- 21st century; Children's stories -- Translations into Hebrew; Pets -- Juvenile fiction; Friendship -- Juvenile fiction; Human-animal relationships -- Juvenile fiction,Children's stories, English -- Translations into Hebrew; Pets -- Juvenile fiction; Friendship -- Juvenile fiction; Human-animal relationships -- Juvenile fiction</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>990049151760205171,990034989930205171</t>
+          <t>990034989930205171,990049151760205171</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1884,12 +1884,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NNL_MUSIC_AL71348238890005171,NNL_ALEPH21282927870005171</t>
+          <t>NNL_ALEPH21282927870005171,NNL_MUSIC_AL71348238890005171</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_MUSIC_AL71348238890005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21282927870005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21282927870005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_MUSIC_AL71348238890005171</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1924,12 +1924,12 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>990034743930205171,997008915936105171</t>
+          <t>997008915936105171,990034743930205171</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>dafshir,book</t>
+          <t>book,dafshir</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -2176,17 +2176,17 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NNL_ALEPH11361294880005171,NNL_ALEPH21243323940005171</t>
+          <t>NNL_ALEPH21243323940005171,NNL_ALEPH11361294880005171</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21243323940005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361294880005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361294880005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21243323940005171</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>אבני בר און, אורית$$Qאבני בר און, אורית,אבני בר און, אורית מחבר$$Qאבני בר און, אורית</t>
+          <t>אבני בר און, אורית מחבר$$Qאבני בר און, אורית,אבני בר און, אורית$$Qאבני בר און, אורית</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2226,7 +2226,7 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -2305,7 +2305,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>מונו הוא לא ארנב : (ואני בכלל לא מענינת לדבר עליו עכשיו) / גור אילני ; אירה הדר ראובן ; [עורכת הספר - רונית רוקאס].,מונו הוא לא ארנב / גור אילני; קריינות: דפנה פרופטה.</t>
+          <t>מונו הוא לא ארנב / גור אילני; קריינות: דפנה פרופטה.,מונו הוא לא ארנב : (ואני בכלל לא מענינת לדבר עליו עכשיו) / גור אילני ; אירה הדר ראובן ; [עורכת הספר - רונית רוקאס].</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2315,7 +2315,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21216598430005171,NNL_ALEPH71270277110005171</t>
+          <t>NNL_ALEPH71270277110005171,NNL_ALEPH21216598430005171</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>תל אביב : טל-מאי ; משכל,תל אביב : iCast</t>
+          <t>תל אביב : iCast,תל אביב : טל-מאי ; משכל</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -2360,7 +2360,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -2605,7 +2605,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>גולדברג, לאה, 1911-1970 מחבר$$Qגולדברג, לאה, 1911-1970,גולדברג, לאה, 1911-1970$$Qגולדברג, לאה, 1911-1970</t>
+          <t>גולדברג, לאה, 1911-1970$$Qגולדברג, לאה, 1911-1970,גולדברג, לאה, 1911-1970 מחבר$$Qגולדברג, לאה, 1911-1970</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
     </row>
@@ -2756,7 +2756,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>זייברט-טל, דנה  $$Qזייברט-טל, דנה,זייברט-טל, דנה  (מתרגם)  $$Qזייברט-טל, דנה</t>
+          <t>זייברט-טל, דנה  (מתרגם)  $$Qזייברט-טל, דנה,זייברט-טל, דנה  $$Qזייברט-טל, דנה</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>לייטנר, ענבל  $$Qלייטנר, ענבל,לייטנר, ענבל  (מאייר)  $$Qלייטנר, ענבל</t>
+          <t>לייטנר, ענבל  (מאייר)  $$Qלייטנר, ענבל,לייטנר, ענבל  $$Qלייטנר, ענבל</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -2870,7 +2870,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>כהן-אסיף, שלומית, 1949- מחבר$$Qכהן-אסיף, שלומית, 1949-,כהן-אסיף, שלומית, 1949-$$Qכהן-אסיף, שלומית, 1949-</t>
+          <t>כהן-אסיף, שלומית, 1949-$$Qכהן-אסיף, שלומית, 1949-,כהן-אסיף, שלומית, 1949- מחבר$$Qכהן-אסיף, שלומית, 1949-</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>55, [1] עמודים : איורים (חלקם צבעוניים) ; 21 ס"מ.,55 עמודים, 3 עמודים לא ממוספרים : איורים צבעוניים ; 20 ס"מ.</t>
+          <t>55 עמודים, 3 עמודים לא ממוספרים : איורים צבעוניים ; 20 ס"מ.,55, [1] עמודים : איורים (חלקם צבעוניים) ; 21 ס"מ.</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -2900,7 +2900,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>990036115890205171,990044075310205171</t>
+          <t>990044075310205171,990036115890205171</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -2917,7 +2917,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ביום שמש בהיר / טלי כוכבי ; איורים - ליאורה גרוסמן ; [עורכת הספר - ליאורה פרידן].,ביום שמש בהיר / טלי כוכבי ; מספרת טלי כוכבי.</t>
+          <t>ביום שמש בהיר / טלי כוכבי ; מספרת טלי כוכבי.,ביום שמש בהיר / טלי כוכבי ; איורים - ליאורה גרוסמן ; [עורכת הספר - ליאורה פרידן].</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -2932,7 +2932,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361379800005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21265726410005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21265726410005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361379800005171</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>אור יהודה : כנרת ; איגואנה,תל אביב : iCast</t>
+          <t>תל אביב : iCast,אור יהודה : כנרת ; איגואנה</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -2977,7 +2977,7 @@
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -2989,22 +2989,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>נל והכתה החדשה / אוש לון; קריינות: אורנה כץ.,נל והכתה החדשה / אוש לון ; איורים - פרנציסקה הארוויי ; מגרמנית - חנה לבנת ; [תרגום - חנה לבנת ; עריכת תרגום - נעמה ברקוביץ' ; עיצוב הספר - אודי טאוב].</t>
+          <t>נל והכתה החדשה / אוש לון ; איורים - פרנציסקה הארוויי ; מגרמנית - חנה לבנת ; [תרגום - חנה לבנת ; עריכת תרגום - נעמה ברקוביץ' ; עיצוב הספר - אודי טאוב].,נל והכתה החדשה / אוש לון; קריינות: אורנה כץ.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>לבנת, חנה, 1951-  $$Qלבנת, חנה, 1951-,כץ, אורנה, 1965-  (דובר)  $$Qכץ, אורנה, 1965-</t>
+          <t>כץ, אורנה, 1965-  (דובר)  $$Qכץ, אורנה, 1965-,לבנת, חנה, 1951-  $$Qלבנת, חנה, 1951-</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21211274580005171,NNL_ALEPH11375550480005171</t>
+          <t>NNL_ALEPH11375550480005171,NNL_ALEPH21211274580005171</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11375550480005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21211274580005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21211274580005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11375550480005171</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3019,7 +3019,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>127 עמודים : איורים (חלקם צבעוניים) ; 21 ס"מ.,1 מקור מקוון.</t>
+          <t>1 מקור מקוון.,127 עמודים : איורים (חלקם צבעוניים) ; 21 ס"מ.</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>[גבעתיים] : רימונים,תל אביב : iCast</t>
+          <t>תל אביב : iCast,[גבעתיים] : רימונים</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -3044,7 +3044,7 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -3197,7 +3197,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21265708570005171,NNL_ALEPH21509602040005171</t>
+          <t>NNL_ALEPH21509602040005171,NNL_ALEPH21265708570005171</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -3212,27 +3212,27 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Dreams -- Juvenile fiction; Zoo animals -- Juvenile fiction; Father and child -- Juvenile fiction; Imagination -- Juvenile fiction; Children's stories, Hebrew -- Translations into Spanish,Children's stories, Hebrew -- 21st century; Zoo animals -- Juvenile fiction; Dreams -- Juvenile fiction</t>
+          <t>Children's stories, Hebrew -- 21st century; Zoo animals -- Juvenile fiction; Dreams -- Juvenile fiction,Dreams -- Juvenile fiction; Zoo animals -- Juvenile fiction; Father and child -- Juvenile fiction; Imagination -- Juvenile fiction; Children's stories, Hebrew -- Translations into Spanish</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[38] עמודים, [6] עמודים מקופלים : איורים צבעוניים ; 29 ס"מ.,38 unnumbered pages : color illustrations ; 28 cm.</t>
+          <t>38 unnumbered pages : color illustrations ; 28 cm.,[38] עמודים, [6] עמודים מקופלים : איורים צבעוניים ; 29 ס"מ.</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>אור יהודה : כנרת, זמורה-ביתן, דביר,México, D.F : Alfaguara Infantil ; Santillana Ediciones Generales</t>
+          <t>México, D.F : Alfaguara Infantil ; Santillana Ediciones Generales,אור יהודה : כנרת, זמורה-ביתן, דביר</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>spa,heb</t>
+          <t>heb,spa</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>990035352810205171,997012399065805171</t>
+          <t>997012399065805171,990035352810205171</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -3259,17 +3259,17 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21219169980005171,NNL_ALEPH11361315990005171</t>
+          <t>NNL_ALEPH11361315990005171,NNL_ALEPH21219169980005171</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361315990005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21219169980005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21219169980005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361315990005171</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>רוזנטל, רוביק, 1945- מחבר$$Qרוזנטל, רוביק, 1945-,רוזנטל, רוביק, 1945- מחבר דובר$$Qרוזנטל, רוביק, 1945-</t>
+          <t>רוזנטל, רוביק, 1945- מחבר דובר$$Qרוזנטל, רוביק, 1945-,רוזנטל, רוביק, 1945- מחבר$$Qרוזנטל, רוביק, 1945-</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -3289,7 +3289,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>20150101,20140101</t>
+          <t>20140101,20150101</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -3321,7 +3321,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>הארנב שרצה להיות עץ / דוידי רוזנפלד; קריינות: דוידי רוזנפלד.,הארנב שרצה להיות עץ / דוידי רוזנפלד ; איורים - מאיה שלייפר ; עורכת הספר - רחלה זנדנבק.</t>
+          <t>הארנב שרצה להיות עץ / דוידי רוזנפלד ; איורים - מאיה שלייפר ; עורכת הספר - רחלה זנדנבק.,הארנב שרצה להיות עץ / דוידי רוזנפלד; קריינות: דוידי רוזנפלד.</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -3331,17 +3331,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>NNL_ALEPH11375553400005171,NNL_ALEPH21224140910005171</t>
+          <t>NNL_ALEPH21224140910005171,NNL_ALEPH11375553400005171</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21224140910005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11375553400005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11375553400005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21224140910005171</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>רוזנפלד, דוידי, 1966-$$Qרוזנפלד, דוידי, 1966-,רוזנטל, רוביק, 1945- מחבר דובר$$Qרוזנטל, רוביק, 1945-</t>
+          <t>רוזנטל, רוביק, 1945- מחבר דובר$$Qרוזנטל, רוביק, 1945-,רוזנפלד, דוידי, 1966-$$Qרוזנפלד, דוידי, 1966-</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -3351,12 +3351,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>[33] עמודים : איורים צבעוניים ; 28 ס"מ.,1 מקור מקוון.</t>
+          <t>1 מקור מקוון.,[33] עמודים : איורים צבעוניים ; 28 ס"מ.</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>20160101,20130101</t>
+          <t>20130101,20160101</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -3594,7 +3594,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>20160101,20130101</t>
+          <t>20130101,20160101</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
@@ -3784,7 +3784,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21187440900005171,NNL_ALEPH11349308370005171</t>
+          <t>NNL_ALEPH11349308370005171,NNL_ALEPH21187440900005171</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3819,7 +3819,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Tel Aviv : הקיבוץ המאוחד,תל אביב : iCast</t>
+          <t>תל אביב : iCast,Tel Aviv : הקיבוץ המאוחד</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -3834,7 +3834,7 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
@@ -4466,7 +4466,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>מתחת שמיים זרועי כוכבים / חנה לבנה ; עריכה - שחר בוגנים.,מתחת שמיים זרועי כוכבים / חנה לבנה; קריינות: חנה לבנה.</t>
+          <t>מתחת שמיים זרועי כוכבים / חנה לבנה; קריינות: חנה לבנה.,מתחת שמיים זרועי כוכבים / חנה לבנה ; עריכה - שחר בוגנים.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -4476,7 +4476,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NNL_ALEPH11375593720005171,NNL_ALEPH21257430670005171</t>
+          <t>NNL_ALEPH21257430670005171,NNL_ALEPH11375593720005171</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -4486,7 +4486,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>ליבנה, חנה, 1950- מחבר דובר$$Qליבנה, חנה, 1950-,ליבנה, חנה, 1950-$$Qליבנה, חנה, 1950-</t>
+          <t>ליבנה, חנה, 1950-$$Qליבנה, חנה, 1950-,ליבנה, חנה, 1950- מחבר דובר$$Qליבנה, חנה, 1950-</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -4600,12 +4600,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ספורו של דוקטור דוליטל / סופר ואויר על ידי יו לופטינג ; מאנגלית - חנה לבנת.,ספורו של דוקטור דוליטל : שהוא תולדות חייו המוזרים בביתו והרפתקאותיו המדהימות באזורים מרחקים שלא נודעו עד כה / יו לופטינג ; תרגמה עטרה אופק.</t>
+          <t>ספורו של דוקטור דוליטל : שהוא תולדות חייו המוזרים בביתו והרפתקאותיו המדהימות באזורים מרחקים שלא נודעו עד כה / יו לופטינג ; תרגמה עטרה אופק.,ספורו של דוקטור דוליטל / סופר ואויר על ידי יו לופטינג ; מאנגלית - חנה לבנת.</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>לבנת, חנה, 1951-  $$Qלבנת, חנה, 1951-,אופק, עטרה, 1953-  $$Qאופק, עטרה, 1953-</t>
+          <t>אופק, עטרה, 1953-  $$Qאופק, עטרה, 1953-,לבנת, חנה, 1951-  $$Qלבנת, חנה, 1951-</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -4615,7 +4615,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21277373690005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21232191800005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21232191800005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21277373690005171</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -4625,7 +4625,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Children's stories, English -- Translations into Hebrew,Children's stories, English -- 20th century; Children's stories -- Translations into Hebrew; Animals -- Juvenile fiction</t>
+          <t>Children's stories, English -- 20th century; Children's stories -- Translations into Hebrew; Animals -- Juvenile fiction,Children's stories, English -- Translations into Hebrew</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>990017709250205171,990035376550205171</t>
+          <t>990035376550205171,990017709250205171</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -5373,7 +5373,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pressler, Mirjam  $$QPressler, Mirjam,סדן, שלמה, 1951-  (דובר)  $$Qסדן, שלמה, 1951-</t>
+          <t>סדן, שלמה, 1951-  (דובר)  $$Qסדן, שלמה, 1951-,Pressler, Mirjam  $$QPressler, Mirjam</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -5413,7 +5413,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -5678,12 +5678,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>יוגב, רבקה  (עורך)  $$Qיוגב, רבקה,ברגמן, אורית, 1966-  (דובר)  $$Qברגמן, אורית, 1966-</t>
+          <t>ברגמן, אורית, 1966-  (דובר)  $$Qברגמן, אורית, 1966-,יוגב, רבקה  (עורך)  $$Qיוגב, רבקה</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ברגמן, אורית, 1966- מחבר$$Qברגמן, אורית, 1966-,ברגמן, אורית, 1966- מחבר דובר$$Qברגמן, אורית, 1966-</t>
+          <t>ברגמן, אורית, 1966- מחבר דובר$$Qברגמן, אורית, 1966-,ברגמן, אורית, 1966- מחבר$$Qברגמן, אורית, 1966-</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -5772,7 +5772,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>הלב של ליליום / עמי גדליה ; מספרת יעל אייזנברג.,הלב של ליליום / עמי גדליה ; [עורכת הספר - מיכל פז-קלפ].</t>
+          <t>הלב של ליליום / עמי גדליה ; [עורכת הספר - מיכל פז-קלפ].,הלב של ליליום / עמי גדליה ; מספרת יעל אייזנברג.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -5787,12 +5787,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21234718910005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361297760005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361297760005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21234718910005171</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>גדליה, עמי, 1952-$$Qגדליה, עמי, 1952-,גדליה, עמי, 1952- מחבר$$Qגדליה, עמי, 1952-</t>
+          <t>גדליה, עמי, 1952- מחבר$$Qגדליה, עמי, 1952-,גדליה, עמי, 1952-$$Qגדליה, עמי, 1952-</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -5827,12 +5827,12 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>990035737920205171,990039034420205171</t>
+          <t>990039034420205171,990035737920205171</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -6050,7 +6050,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>דשנר, ג'יימס, 1972- מחבר$$Qדשנר, ג'יימס, 1972-,דשנר, ג'יימס, 1972-$$Qדשנר, ג'יימס, 1972-</t>
+          <t>דשנר, ג'יימס, 1972-$$Qדשנר, ג'יימס, 1972-,דשנר, ג'יימס, 1972- מחבר$$Qדשנר, ג'יימס, 1972-</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -6127,7 +6127,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>תל-אביב : קרן הוצאה לאור,תל אביב : iCast</t>
+          <t>תל אביב : iCast,תל-אביב : קרן הוצאה לאור</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -6142,19 +6142,19 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>$$VThe National Library of Israel$$ONNL_ALEPH21168565340005171,The National Library of Israel</t>
+          <t>The National Library of Israel,$$VThe National Library of Israel$$ONNL_ALEPH21168565340005171</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>מנדלה</t>
+          <t>[כנס לזכרו של הסופר מנדלה מוכר הספרים].</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -6172,19 +6172,14 @@
           <t>גלס, ערי, 1897-1973 צלם</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>مانديلا، نيلسون; Mandela, Nelson, 1918-2013 -- Fiction; South Africa -- Politics and government -- 20th century; South Africa -- Race relations</t>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE26402618</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
           <t>1 מקור מקוון..</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>19470101</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -6231,7 +6226,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE36242825,https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE51473265</t>
+          <t>https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE51473265,https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE36242825</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -6246,7 +6241,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>בני-ברק : הקיבוץ המאוחד - ספרית הפועלים,תל אביב : iCast</t>
+          <t>תל אביב : iCast,בני-ברק : הקיבוץ המאוחד - ספרית הפועלים</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -6256,7 +6251,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>$$VThe National Library of Israel$$ONNL_ALEPH21294822100005171,The National Library of Israel</t>
+          <t>The National Library of Israel,$$VThe National Library of Israel$$ONNL_ALEPH21294822100005171</t>
         </is>
       </c>
     </row>
@@ -6268,12 +6263,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ליפשיץ, אפרת  (דובר)  $$Qליפשיץ, אפרת,גלברט-אבני, עפרה, 1947-  (עורך)  $$Qגלברט-אבני, עפרה, 1947-</t>
+          <t>גלברט-אבני, עפרה, 1947-  (עורך)  $$Qגלברט-אבני, עפרה, 1947-,ליפשיץ, אפרת  (דובר)  $$Qליפשיץ, אפרת</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21284077860005171,NNL_ALEPH11375553340005171</t>
+          <t>NNL_ALEPH11375553340005171,NNL_ALEPH21284077860005171</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -6303,12 +6298,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>20170101,20140101</t>
+          <t>20140101,20170101</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>תל אביב : משכל,תל אביב : iCast</t>
+          <t>תל אביב : iCast,תל אביב : משכל</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -6318,12 +6313,12 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>990037051250205171,990048842900205171</t>
+          <t>990048842900205171,990037051250205171</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -6821,7 +6816,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>https://nli.alma.exlibrisgroup.com/view/delivery/thumbnail/12303989520005171,https://nli.alma.exlibrisgroup.com/view/delivery/thumbnail/12303425940005171</t>
+          <t>https://nli.alma.exlibrisgroup.com/view/delivery/thumbnail/12303425940005171,https://nli.alma.exlibrisgroup.com/view/delivery/thumbnail/12303989520005171</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -6934,7 +6929,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Pressler, Mirjam  $$QPressler, Mirjam,סדן, שלמה, 1951-  (דובר)  $$Qסדן, שלמה, 1951-</t>
+          <t>סדן, שלמה, 1951-  (דובר)  $$Qסדן, שלמה, 1951-,Pressler, Mirjam  $$QPressler, Mirjam</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -6974,7 +6969,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -7187,7 +7182,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -7204,12 +7199,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>יוגב, רבקה  (עורך)  $$Qיוגב, רבקה,ברגמן, אורית, 1966-  (דובר)  $$Qברגמן, אורית, 1966-</t>
+          <t>ברגמן, אורית, 1966-  (דובר)  $$Qברגמן, אורית, 1966-,יוגב, רבקה  (עורך)  $$Qיוגב, רבקה</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ברגמן, אורית, 1966- מחבר$$Qברגמן, אורית, 1966-,ברגמן, אורית, 1966- מחבר דובר$$Qברגמן, אורית, 1966-</t>
+          <t>ברגמן, אורית, 1966- מחבר דובר$$Qברגמן, אורית, 1966-,ברגמן, אורית, 1966- מחבר$$Qברגמן, אורית, 1966-</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -7298,7 +7293,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>הלב של ליליום / עמי גדליה ; מספרת יעל אייזנברג.,הלב של ליליום / עמי גדליה ; [עורכת הספר - מיכל פז-קלפ].</t>
+          <t>הלב של ליליום / עמי גדליה ; [עורכת הספר - מיכל פז-קלפ].,הלב של ליליום / עמי גדליה ; מספרת יעל אייזנברג.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -7313,12 +7308,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21234718910005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361297760005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH11361297760005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21234718910005171</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>גדליה, עמי, 1952-$$Qגדליה, עמי, 1952-,גדליה, עמי, 1952- מחבר$$Qגדליה, עמי, 1952-</t>
+          <t>גדליה, עמי, 1952- מחבר$$Qגדליה, עמי, 1952-,גדליה, עמי, 1952-$$Qגדליה, עמי, 1952-</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -7353,12 +7348,12 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>990035737920205171,990039034420205171</t>
+          <t>990039034420205171,990035737920205171</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
@@ -7576,7 +7571,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>דשנר, ג'יימס, 1972- מחבר$$Qדשנר, ג'יימס, 1972-,דשנר, ג'יימס, 1972-$$Qדשנר, ג'יימס, 1972-</t>
+          <t>דשנר, ג'יימס, 1972-$$Qדשנר, ג'יימס, 1972-,דשנר, ג'יימס, 1972- מחבר$$Qדשנר, ג'יימס, 1972-</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -7653,7 +7648,7 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>תל-אביב : קרן הוצאה לאור,תל אביב : iCast</t>
+          <t>תל אביב : iCast,תל-אביב : קרן הוצאה לאור</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -7668,19 +7663,19 @@
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>$$VThe National Library of Israel$$ONNL_ALEPH21168565340005171,The National Library of Israel</t>
+          <t>The National Library of Israel,$$VThe National Library of Israel$$ONNL_ALEPH21168565340005171</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>מנדלה</t>
+          <t>[כנס לזכרו של הסופר מנדלה מוכר הספרים].</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -7698,19 +7693,14 @@
           <t>גלס, ערי, 1897-1973 צלם</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>مانديلا، نيلسون; Mandela, Nelson, 1918-2013 -- Fiction; South Africa -- Politics and government -- 20th century; South Africa -- Race relations</t>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE26402618</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
           <t>1 מקור מקוון..</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>19470101</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
@@ -7757,7 +7747,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE36242825,https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE51473265</t>
+          <t>https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE51473265,https://rosetta.nli.org.il/delivery/DeliveryManagerServlet?dps_func=thumbnail&amp;dps_pid=IE36242825</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -7772,7 +7762,7 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>בני-ברק : הקיבוץ המאוחד - ספרית הפועלים,תל אביב : iCast</t>
+          <t>תל אביב : iCast,בני-ברק : הקיבוץ המאוחד - ספרית הפועלים</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -7782,7 +7772,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>$$VThe National Library of Israel$$ONNL_ALEPH21294822100005171,The National Library of Israel</t>
+          <t>The National Library of Israel,$$VThe National Library of Israel$$ONNL_ALEPH21294822100005171</t>
         </is>
       </c>
     </row>
@@ -7794,12 +7784,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ליפשיץ, אפרת  (דובר)  $$Qליפשיץ, אפרת,גלברט-אבני, עפרה, 1947-  (עורך)  $$Qגלברט-אבני, עפרה, 1947-</t>
+          <t>גלברט-אבני, עפרה, 1947-  (עורך)  $$Qגלברט-אבני, עפרה, 1947-,ליפשיץ, אפרת  (דובר)  $$Qליפשיץ, אפרת</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21284077860005171,NNL_ALEPH11375553340005171</t>
+          <t>NNL_ALEPH11375553340005171,NNL_ALEPH21284077860005171</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -7829,12 +7819,12 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>20170101,20140101</t>
+          <t>20140101,20170101</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>תל אביב : משכל,תל אביב : iCast</t>
+          <t>תל אביב : iCast,תל אביב : משכל</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
@@ -7844,12 +7834,12 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>990037051250205171,990048842900205171</t>
+          <t>990048842900205171,990037051250205171</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -8418,7 +8408,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>לא מפסיקים אהבה באמצע / ליאור אנגלמן ; [עורכת הספר - נועה מנהיים].,לא מפסיקים אהבה באמצע / ליאור אנגלמן ; מספר ליאור אנגלמן.</t>
+          <t>לא מפסיקים אהבה באמצע / ליאור אנגלמן ; מספר ליאור אנגלמן.,לא מפסיקים אהבה באמצע / ליאור אנגלמן ; [עורכת הספר - נועה מנהיים].</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -8428,7 +8418,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21237983750005171,NNL_ALEPH11361330460005171</t>
+          <t>NNL_ALEPH11361330460005171,NNL_ALEPH21237983750005171</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -8473,12 +8463,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>990039033150205171,990036687830205171</t>
+          <t>990036687830205171,990039033150205171</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -8505,7 +8495,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH71270289320005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21294821790005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21294821790005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH71270289320005171</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -8525,7 +8515,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Tel Aviv : הקיבוץ המאוחד,תל אביב : iCast</t>
+          <t>תל אביב : iCast,Tel Aviv : הקיבוץ המאוחד</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -8535,12 +8525,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>990035422990205171,990048968400205171</t>
+          <t>990048968400205171,990035422990205171</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -9105,7 +9095,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ילדה רגילה לגמרי / רועי ישורון ; [עורכת הספר - שרי גוטמן].,ילדה רגילה לגמרי / רועי ישורון ; מספר רועי ישורון.</t>
+          <t>ילדה רגילה לגמרי / רועי ישורון ; מספר רועי ישורון.,ילדה רגילה לגמרי / רועי ישורון ; [עורכת הספר - שרי גוטמן].</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -9115,7 +9105,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>NNL_ALEPH11361310730005171,NNL_ALEPH21172588270005171</t>
+          <t>NNL_ALEPH21172588270005171,NNL_ALEPH11361310730005171</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -9145,7 +9135,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>תל אביב : אחוזת בית,תל אביב : iCast</t>
+          <t>תל אביב : iCast,תל אביב : אחוזת בית</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -9155,12 +9145,12 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>990036325750205171,990039033900205171</t>
+          <t>990039033900205171,990036325750205171</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -9182,7 +9172,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>https://nli.alma.exlibrisgroup.com/view/delivery/thumbnail/12302749940005171,https://nli.alma.exlibrisgroup.com/view/delivery/thumbnail/12413035440005171</t>
+          <t>https://nli.alma.exlibrisgroup.com/view/delivery/thumbnail/12413035440005171,https://nli.alma.exlibrisgroup.com/view/delivery/thumbnail/12302749940005171</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -9276,7 +9266,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>20150101,20120101</t>
+          <t>20120101,20150101</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
@@ -9365,12 +9355,12 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>אלכסנדרוביץ', זאב, 1905-1992 צלם,מקיואן, איאן, 1948-$$Qמקיואן, איאן, 1948-</t>
+          <t>מקיואן, איאן, 1948-$$Qמקיואן, איאן, 1948-,אלכסנדרוביץ', זאב, 1905-1992 צלם</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Tokyo (Japan) -- Photographs,Fiction -- Translations into Hebrew; Women spies -- Fiction; Cold War -- Fiction; Intelligence service -- Great Britain -- Fiction</t>
+          <t>Fiction -- Translations into Hebrew; Women spies -- Fiction; Cold War -- Fiction; Intelligence service -- Great Britain -- Fiction,Tokyo (Japan) -- Photographs</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -9395,7 +9385,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>zxx,heb</t>
+          <t>heb,zxx</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -9479,7 +9469,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Bergen-Belsen (Concentration camp) -- Fiction; Hebrew fiction -- Translations into English; Jewish families -- Libya -- Fiction; Jews -- Libya -- Banghāzī -- Fiction; Holocaust, Jewish (1939-1945) -- Africa, North -- Fiction,Bergen-Belsen (Concentration camp) -- Fiction; Jewish families -- Libya -- Fiction; Jews -- Libya -- Banghāzī -- Fiction; Holocaust, Jewish (1939-1945) -- Africa, North -- Fiction</t>
+          <t>Bergen-Belsen (Concentration camp) -- Fiction; Jewish families -- Libya -- Fiction; Jews -- Libya -- Banghāzī -- Fiction; Holocaust, Jewish (1939-1945) -- Africa, North -- Fiction,Bergen-Belsen (Concentration camp) -- Fiction; Hebrew fiction -- Translations into English; Jewish families -- Libya -- Fiction; Jews -- Libya -- Banghāzī -- Fiction; Holocaust, Jewish (1939-1945) -- Africa, North -- Fiction</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -9509,7 +9499,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>$$VThe National Library of Israel$$ONNL_ALEPH21265653910005171,The National Library of Israel</t>
+          <t>The National Library of Israel,$$VThe National Library of Israel$$ONNL_ALEPH21265653910005171</t>
         </is>
       </c>
     </row>
@@ -9815,7 +9805,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>לא מפסיקים אהבה באמצע / ליאור אנגלמן ; [עורכת הספר - נועה מנהיים].,לא מפסיקים אהבה באמצע / ליאור אנגלמן ; מספר ליאור אנגלמן.</t>
+          <t>לא מפסיקים אהבה באמצע / ליאור אנגלמן ; מספר ליאור אנגלמן.,לא מפסיקים אהבה באמצע / ליאור אנגלמן ; [עורכת הספר - נועה מנהיים].</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -9825,7 +9815,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NNL_ALEPH21237983750005171,NNL_ALEPH11361330460005171</t>
+          <t>NNL_ALEPH11361330460005171,NNL_ALEPH21237983750005171</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -9870,12 +9860,12 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>990039033150205171,990036687830205171</t>
+          <t>990036687830205171,990039033150205171</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -9902,7 +9892,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH71270289320005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21294821790005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21294821790005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH71270289320005171</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -9922,7 +9912,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Tel Aviv : הקיבוץ המאוחד,תל אביב : iCast</t>
+          <t>תל אביב : iCast,Tel Aviv : הקיבוץ המאוחד</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -9932,12 +9922,12 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>990035422990205171,990048968400205171</t>
+          <t>990048968400205171,990035422990205171</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -9949,7 +9939,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Руководство к действию на ближайшие дни / Йоав Блум ; [перевод с иврита Александры Полян].,המדריך לימים הקרובים / יואב בלום ; [עורכת הספר - שירה חדד].</t>
+          <t>המדריך לימים הקרובים / יואב בלום ; [עורכת הספר - שירה חדד].,Руководство к действию на ближайшие дни / Йоав Блум ; [перевод с иврита Александры Полян].</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -9964,12 +9954,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21237982660005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21243170670005171</t>
+          <t>https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21243170670005171,https://merhav.nli.org.il/primo-explore/sourceRecord?vid=NLI&amp;docId=NNL_ALEPH21237982660005171</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>בלום, יואב, 1978-$$Qבלום, יואב, 1978-,Йоав Блум$$QБлум, Йоав</t>
+          <t>Йоав Блум$$QБлум, Йоав,בלום, יואב, 1978-$$Qבלום, יואב, 1978-</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -9984,22 +9974,22 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>20140101,20190101</t>
+          <t>20190101,20140101</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Москва : Иностранка; Азбука-Аттикус,ירושלים : כתר</t>
+          <t>ירושלים : כתר,Москва : Иностранка; Азбука-Аттикус</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>rus,heb</t>
+          <t>heb,rus</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>990036687890205171,990050486350205171</t>
+          <t>990050486350205171,990036687890205171</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -10440,7 +10430,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ילדה רגילה לגמרי / רועי ישורון ; [עורכת הספר - שרי גוטמן].,ילדה רגילה לגמרי / רועי ישורון ; מספר רועי ישורון.</t>
+          <t>ילדה רגילה לגמרי / רועי ישורון ; מספר רועי ישורון.,ילדה רגילה לגמרי / רועי ישורון ; [עורכת הספר - שרי גוטמן].</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -10450,7 +10440,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>NNL_ALEPH11361310730005171,NNL_ALEPH21172588270005171</t>
+          <t>NNL_ALEPH21172588270005171,NNL_ALEPH11361310730005171</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -10480,7 +10470,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>תל אביב : אחוזת בית,תל אביב : iCast</t>
+          <t>תל אביב : iCast,תל אביב : אחוזת בית</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -10490,12 +10480,12 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>990036325750205171,990039033900205171</t>
+          <t>990039033900205171,990036325750205171</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>book,audio</t>
+          <t>audio,book</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -10522,7 +10512,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>20150101,20120101</t>
+          <t>20120101,20150101</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">

</xml_diff>